<commit_message>
Tweaked rail calculation and outputs
</commit_message>
<xml_diff>
--- a/Racking Rails Counts.xlsx
+++ b/Racking Rails Counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryley\Github\racking-builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E514CE70-D969-439F-9544-CC155BB06ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7688D02C-C0B1-4269-90AC-349ACDBF69D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26730" yWindow="2745" windowWidth="14115" windowHeight="15435" xr2:uid="{23220582-B46C-4E74-9A12-1D268C5229C5}"/>
+    <workbookView xWindow="35220" yWindow="795" windowWidth="14115" windowHeight="15435" xr2:uid="{23220582-B46C-4E74-9A12-1D268C5229C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4035,7 +4035,7 @@
   <dimension ref="A1:AD61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4093,6 +4093,10 @@
         <f t="shared" ref="F2:F17" si="0">B2*2-C2*$C$1-D2*$D$1</f>
         <v>-34.70866141732283</v>
       </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G16" si="1">FLOOR(SUM(C2:D2)/2,1)+MOD(SUM(C2:D2),2)*2</f>
+        <v>2</v>
+      </c>
       <c r="H2" t="s">
         <v>11</v>
       </c>
@@ -4102,7 +4106,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B17" si="1">A3*1134/25.4+(A3-1)*5/8+8</f>
+        <f t="shared" ref="B3:B17" si="2">A3*1134/25.4+(A3-1)*5/8+8</f>
         <v>97.91633858267717</v>
       </c>
       <c r="C3" s="2">
@@ -4117,6 +4121,10 @@
       <c r="F3" s="2">
         <f t="shared" si="0"/>
         <v>-84.16732283464566</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
@@ -4127,7 +4135,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>143.18700787401576</v>
       </c>
       <c r="C4" s="2">
@@ -4142,6 +4150,10 @@
       <c r="F4" s="2">
         <f t="shared" si="0"/>
         <v>-38.625984251968475</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -4152,7 +4164,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>188.45767716535434</v>
       </c>
       <c r="C5" s="2">
@@ -4167,6 +4179,10 @@
       <c r="F5" s="2">
         <f t="shared" si="0"/>
         <v>-43.084645669291319</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -4177,7 +4193,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>233.72834645669292</v>
       </c>
       <c r="C6" s="2">
@@ -4192,6 +4208,10 @@
       <c r="F6" s="2">
         <f t="shared" si="0"/>
         <v>-42.543307086614163</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
@@ -4202,7 +4222,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>278.99901574803152</v>
       </c>
       <c r="C7" s="2">
@@ -4217,6 +4237,10 @@
       <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>-2.0019685039369506</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="H7" t="s">
         <v>9</v>
@@ -4227,7 +4251,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>324.26968503937007</v>
       </c>
       <c r="C8" s="2">
@@ -4242,6 +4266,10 @@
       <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>-1.4606299212598515</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
@@ -4252,7 +4280,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>369.54035433070868</v>
       </c>
       <c r="C9" s="2">
@@ -4267,6 +4295,10 @@
       <c r="F9" s="2">
         <f t="shared" si="0"/>
         <v>-0.91929133858263867</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4274,7 +4306,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>414.81102362204729</v>
       </c>
       <c r="C10" s="2">
@@ -4289,6 +4321,10 @@
       <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>-50.377952755905426</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4296,7 +4332,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>460.08169291338584</v>
       </c>
       <c r="C11" s="2">
@@ -4311,6 +4347,10 @@
       <c r="F11" s="2">
         <f t="shared" si="0"/>
         <v>-4.8366141732283268</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4318,7 +4358,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>505.35236220472444</v>
       </c>
       <c r="C12" s="2">
@@ -4333,6 +4373,10 @@
       <c r="F12" s="2">
         <f t="shared" si="0"/>
         <v>-9.295275590551114</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4340,7 +4384,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>550.62303149606305</v>
       </c>
       <c r="C13" s="2">
@@ -4355,6 +4399,10 @@
       <c r="F13" s="2">
         <f t="shared" si="0"/>
         <v>-8.7539370078739012</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4362,7 +4410,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>595.8937007874016</v>
       </c>
       <c r="C14" s="2">
@@ -4377,6 +4425,10 @@
       <c r="F14" s="2">
         <f t="shared" si="0"/>
         <v>-58.212598425196802</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4384,7 +4436,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>641.16437007874015</v>
       </c>
       <c r="C15" s="2">
@@ -4399,6 +4451,10 @@
       <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>-12.671259842519703</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4406,7 +4462,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>686.43503937007881</v>
       </c>
       <c r="C16" s="2">
@@ -4421,6 +4477,10 @@
       <c r="F16" s="2">
         <f t="shared" si="0"/>
         <v>-17.129921259842376</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -4428,7 +4488,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>731.70570866141736</v>
       </c>
       <c r="C17" s="2">
@@ -4443,6 +4503,10 @@
       <c r="F17" s="2">
         <f t="shared" si="0"/>
         <v>-16.588582677165277</v>
+      </c>
+      <c r="G17">
+        <f>FLOOR(SUM(C17:D17)/2,1)+MOD(SUM(C17:D17),2)*2</f>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -4464,6 +4528,12 @@
       <c r="F19" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -4483,8 +4553,14 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" ref="F20:F27" si="2">B20*2-C20*$C$19-D20*$D$19</f>
+        <f t="shared" ref="F20:F27" si="3">B20*2-C20*$C$19-D20*$D$19</f>
         <v>-4.118110236220474</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -4492,7 +4568,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B27" si="3">A21*2094/25.4+(A21-1)*5/8+8</f>
+        <f t="shared" ref="B21:B27" si="4">A21*2094/25.4+(A21-1)*5/8+8</f>
         <v>173.50688976377953</v>
       </c>
       <c r="C21" s="2">
@@ -4505,8 +4581,14 @@
         <v>0</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-22.986220472440948</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -4514,7 +4596,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>256.57283464566933</v>
       </c>
       <c r="C22" s="2">
@@ -4527,8 +4609,14 @@
         <v>2</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-41.854330708661337</v>
+      </c>
+      <c r="G22" s="2">
+        <v>4</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -4536,7 +4624,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>339.63877952755905</v>
       </c>
       <c r="C23" s="2">
@@ -4549,8 +4637,14 @@
         <v>2</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-60.722440944881896</v>
+      </c>
+      <c r="G23" s="2">
+        <v>5</v>
+      </c>
+      <c r="H23" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -4558,7 +4652,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>422.70472440944883</v>
       </c>
       <c r="C24" s="2">
@@ -4571,8 +4665,14 @@
         <v>4</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-79.590551181102342</v>
+      </c>
+      <c r="G24" s="2">
+        <v>6</v>
+      </c>
+      <c r="H24" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -4580,7 +4680,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>505.77066929133861</v>
       </c>
       <c r="C25" s="2">
@@ -4593,8 +4693,14 @@
         <v>4</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-8.4586614173227872</v>
+      </c>
+      <c r="G25" s="2">
+        <v>7</v>
+      </c>
+      <c r="H25" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -4602,7 +4708,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>588.83661417322833</v>
       </c>
       <c r="C26" s="2">
@@ -4615,8 +4721,14 @@
         <v>6</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-72.326771653543346</v>
+      </c>
+      <c r="G26" s="2">
+        <v>8</v>
+      </c>
+      <c r="H26" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -4624,7 +4736,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>671.9025590551181</v>
       </c>
       <c r="C27" s="2">
@@ -4637,7 +4749,7 @@
         <v>6</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-46.194881889763792</v>
       </c>
     </row>
@@ -4879,15 +4991,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034C8E3736A37DC438055067A7FE579C0" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4543a09f24a63ff0e92405460d34b6aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f008cd8d-fe66-4e7d-904b-0176267cc631" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2b9b060166466cfa73c3f7b3d4f8e59" ns3:_="">
     <xsd:import namespace="f008cd8d-fe66-4e7d-904b-0176267cc631"/>
@@ -5045,6 +5148,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5052,14 +5164,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B902530-103C-4A33-94D2-9BAA675D808D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFE3A5CE-BB28-4674-ADCC-0E15CFDD946E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5073,6 +5177,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B902530-103C-4A33-94D2-9BAA675D808D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>